<commit_message>
EPBDS-11841 Incorrect error message is presented for the SmartLookup with the empty columns
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8343_HC_Titles.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8343_HC_Titles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-8343\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655ACF9B-EADF-4AFC-8A46-75E8961CD87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D220B6-D36E-493B-8B64-6F88BA217811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43320" yWindow="1860" windowWidth="18830" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3260" yWindow="2450" windowWidth="17940" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -285,10 +285,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -631,7 +631,7 @@
   <dimension ref="B5:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H118" sqref="H118"/>
+      <selection activeCell="H107" sqref="H107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
@@ -656,13 +656,13 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="13"/>
+      <c r="E6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
+      <c r="B7" s="12"/>
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -711,13 +711,13 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
@@ -777,7 +777,7 @@
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C19" t="s">
@@ -786,13 +786,13 @@
       <c r="D19" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="13"/>
+      <c r="E19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
+      <c r="B20" s="12"/>
       <c r="C20" t="s">
         <v>0</v>
       </c>
@@ -841,13 +841,13 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
@@ -960,7 +960,7 @@
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C40" t="s">
@@ -969,13 +969,13 @@
       <c r="D40" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F40" s="13"/>
+      <c r="E40" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="12"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="13"/>
+      <c r="B41" s="12"/>
       <c r="C41" t="s">
         <v>46</v>
       </c>
@@ -1024,12 +1024,12 @@
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
@@ -1089,7 +1089,7 @@
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C53" t="s">
@@ -1098,13 +1098,13 @@
       <c r="D53" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F53" s="13"/>
+      <c r="E53" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F53" s="12"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="13"/>
+      <c r="B54" s="12"/>
       <c r="C54" t="s">
         <v>40</v>
       </c>
@@ -1153,12 +1153,12 @@
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="s">
@@ -1224,7 +1224,7 @@
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C70" t="s">
@@ -1233,13 +1233,13 @@
       <c r="D70" t="s">
         <v>2</v>
       </c>
-      <c r="E70" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F70" s="13"/>
+      <c r="E70" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" s="12"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="13"/>
+      <c r="B71" s="12"/>
       <c r="C71" t="s">
         <v>0</v>
       </c>
@@ -1352,13 +1352,13 @@
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="12" t="s">
+      <c r="B86" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="9" t="s">
@@ -1418,16 +1418,16 @@
       <c r="C94" s="1"/>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="13" t="s">
+      <c r="B95" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C95" s="13"/>
-      <c r="D95" s="13"/>
-      <c r="E95" s="13"/>
-      <c r="F95" s="13"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="13" t="s">
+      <c r="B96" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C96" t="s">
@@ -1436,13 +1436,13 @@
       <c r="D96" t="s">
         <v>2</v>
       </c>
-      <c r="E96" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F96" s="13"/>
+      <c r="E96" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F96" s="12"/>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="13"/>
+      <c r="B97" s="12"/>
       <c r="C97" t="s">
         <v>0</v>
       </c>
@@ -1491,13 +1491,13 @@
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" s="12" t="s">
+      <c r="B103" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C103" s="12"/>
-      <c r="D103" s="12"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="11" t="s">
@@ -1557,20 +1557,23 @@
       <c r="C112" s="1"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B113" s="13" t="s">
+      <c r="B113" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C113" s="1"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" s="13"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B115" s="13" t="s">
+      <c r="B115" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C115" t="s">
@@ -1579,13 +1582,13 @@
       <c r="D115" t="s">
         <v>2</v>
       </c>
-      <c r="E115" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F115" s="13"/>
+      <c r="E115" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F115" s="12"/>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B116" s="13"/>
+      <c r="B116" s="12"/>
       <c r="C116" t="s">
         <v>0</v>
       </c>
@@ -1634,13 +1637,13 @@
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="12" t="s">
+      <c r="B122" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C122" s="12"/>
-      <c r="D122" s="12"/>
-      <c r="E122" s="12"/>
-      <c r="F122" s="12"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="11" t="s">
@@ -1694,30 +1697,34 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="27">
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B86:F86"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="E70:F70"/>
     <mergeCell ref="B115:B116"/>
     <mergeCell ref="E115:F115"/>
     <mergeCell ref="B113:B114"/>
     <mergeCell ref="B122:F122"/>
     <mergeCell ref="B96:B97"/>
     <mergeCell ref="E96:F96"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="B103:F103"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>